<commit_message>
implemented status column to TransactionData and items for future workbook output
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature_Workspace\uipath-automation-5\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-8\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D69477E-C6A9-4FCD-AA48-C05A24BCA84C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4364BD9-7D0A-4BE2-89EA-1C7783EF84B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1410" windowWidth="27420" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -140,6 +140,33 @@
   </si>
   <si>
     <t>URL for the login page of RevatureConnect</t>
+  </si>
+  <si>
+    <t>Status_Success</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record successful transaction.</t>
+  </si>
+  <si>
+    <t>Status_Failure</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record failed transaction.</t>
+  </si>
+  <si>
+    <t>Status_Pending</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record pending transaction.</t>
   </si>
 </sst>
 </file>
@@ -526,16 +553,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -584,7 +611,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1619,14 +1646,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1663,7 +1692,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1744,9 +1773,39 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -2733,12 +2792,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
changed process name in Config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-8\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cito\Revature\UiPath Project 3\uipath-automation-8\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4364BD9-7D0A-4BE2-89EA-1C7783EF84B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFAB14A-88FD-4B7F-9A70-8709669DA765}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>ProcessABCQueue</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>Status message for TransactionData to record pending transaction.</t>
+  </si>
+  <si>
+    <t>CreateRevatureConnectBoard</t>
   </si>
 </sst>
 </file>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -601,13 +601,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -616,33 +616,33 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1646,7 +1646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:C15"/>
     </sheetView>
   </sheetViews>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1724,7 +1724,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1746,7 +1746,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1757,7 +1757,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1768,42 +1768,42 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2808,7 +2808,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>